<commit_message>
Please enter the commit message for your changes. Lines starting with '#' will be ignored, and an empty message aborts the commit.
On branch master
Your branch is up to date with 'origin/master'.

Changes to be committed:
	new file:   Projet/Formation/AP2.pdf
	new file:   Projet/Formation/AP2.pptx
	modified:   Tableau_de_synthese_Epreuve_E4.xlsx
	modified:   index.html
</commit_message>
<xml_diff>
--- a/Tableau_de_synthese_Epreuve_E4.xlsx
+++ b/Tableau_de_synthese_Epreuve_E4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walle\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walle\Desktop\Cours\BTS\PORTFOLIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1871B85-B4F5-4A16-A2C1-A2090023CE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5646D275-8884-4F84-9061-F1D2D3E391DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="3360" windowWidth="24686" windowHeight="13123" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5854" yWindow="343" windowWidth="24686" windowHeight="13054" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -102,9 +102,6 @@
     <t>▢ SISR</t>
   </si>
   <si>
-    <t>▢ SLAM</t>
-  </si>
-  <si>
     <t xml:space="preserve">Réalisation en cours de formation
 </t>
   </si>
@@ -141,12 +138,6 @@
     <t>Création d'une application d'utilisateur et d'école avec statistique en  PHP</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Réalisation d'une entreprise fictive</t>
   </si>
   <si>
@@ -154,6 +145,56 @@
   </si>
   <si>
     <t>Mise en  place d'un GLPI</t>
+  </si>
+  <si>
+    <t>ü</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t xml:space="preserve"> þ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> SLAM</t>
+    </r>
+  </si>
+  <si>
+    <t>11/04/2022 au 27/04/2022</t>
+  </si>
+  <si>
+    <t>13/09/2021 au 18/09/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/05/2022 au 14/05/2022 </t>
+  </si>
+  <si>
+    <t>15/04/2022 au 15/06/2022</t>
+  </si>
+  <si>
+    <t>10/01/2022 au 25/02/2022</t>
+  </si>
+  <si>
+    <t>Répondre aux besions de diffarents services demandés</t>
+  </si>
+  <si>
+    <t>09/05/2022 au  10/06/2022</t>
+  </si>
+  <si>
+    <t>Création d'une appication légère avec API</t>
+  </si>
+  <si>
+    <t>21/10/2022 au</t>
   </si>
 </sst>
 </file>
@@ -163,7 +204,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -220,6 +261,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="28"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -620,7 +685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -673,8 +738,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -742,14 +828,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1095,11 +1175,11 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.84375" defaultRowHeight="12.45"/>
   <cols>
     <col min="1" max="1" width="71.3828125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.84375" style="1" customWidth="1"/>
@@ -1111,85 +1191,85 @@
     <col min="44" max="16384" width="10.84375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:43" ht="40" customHeight="1">
+      <c r="A1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1">
+      <c r="A2" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="1:43" ht="40" customHeight="1">
+      <c r="A3" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="21"/>
-    </row>
-    <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-    </row>
-    <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="47"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+    <row r="4" spans="1:43" ht="40" customHeight="1">
+      <c r="A4" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>22</v>
+      <c r="H4" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1">
+      <c r="A5" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1">
+      <c r="A6" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>0</v>
@@ -1210,30 +1290,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="43" t="s">
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1">
+      <c r="A7" s="27"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="19" t="s">
         <v>14</v>
       </c>
       <c r="I7"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7"/>
@@ -1267,17 +1347,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="24"/>
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="17.600000000000001">
+      <c r="A8" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1314,20 +1394,22 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="14" t="s">
-        <v>29</v>
-      </c>
       <c r="D9" s="14"/>
-      <c r="E9" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>30</v>
+      <c r="E9" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
@@ -1367,18 +1449,20 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>34</v>
+      </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="15" t="s">
-        <v>29</v>
+      <c r="H10" s="48" t="s">
+        <v>31</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1416,18 +1500,22 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="14" t="s">
-        <v>29</v>
+      <c r="D11" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="G11" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="H11" s="15"/>
       <c r="I11"/>
       <c r="J11"/>
@@ -1465,15 +1553,23 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>39</v>
+      </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
+      <c r="G12" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>31</v>
+      </c>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1510,14 +1606,24 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>41</v>
+      </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="E13" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="H13" s="15"/>
       <c r="I13"/>
       <c r="J13"/>
@@ -1555,7 +1661,7 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A14" s="9"/>
       <c r="B14" s="8"/>
       <c r="C14" s="14"/>
@@ -1600,7 +1706,7 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A15" s="9"/>
       <c r="B15" s="8"/>
       <c r="C15" s="14"/>
@@ -1645,7 +1751,7 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A16" s="9"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14"/>
@@ -1690,7 +1796,7 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A17" s="9"/>
       <c r="B17" s="8"/>
       <c r="C17" s="14"/>
@@ -1735,7 +1841,7 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A18" s="9"/>
       <c r="B18" s="8"/>
       <c r="C18" s="14"/>
@@ -1780,17 +1886,17 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A19" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="27"/>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="17.600000000000001">
+      <c r="A19" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1827,17 +1933,21 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="14"/>
+        <v>26</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
-      <c r="G20" s="14" t="s">
-        <v>29</v>
+      <c r="G20" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="H20" s="15"/>
       <c r="I20"/>
@@ -1876,13 +1986,15 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -1925,7 +2037,7 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A22" s="9"/>
       <c r="B22" s="8"/>
       <c r="C22" s="14"/>
@@ -1970,7 +2082,7 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A23" s="9"/>
       <c r="B23" s="8"/>
       <c r="C23" s="14"/>
@@ -2015,7 +2127,7 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A24" s="9"/>
       <c r="B24" s="8"/>
       <c r="C24" s="14"/>
@@ -2060,7 +2172,7 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A25" s="9"/>
       <c r="B25" s="8"/>
       <c r="C25" s="14"/>
@@ -2105,7 +2217,7 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A26" s="9"/>
       <c r="B26" s="8"/>
       <c r="C26" s="14"/>
@@ -2150,17 +2262,17 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A27" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="27"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="17.600000000000001">
+      <c r="A27" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2197,7 +2309,7 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A28" s="9"/>
       <c r="B28" s="8"/>
       <c r="C28" s="14"/>
@@ -2242,7 +2354,7 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A29" s="9"/>
       <c r="B29" s="8"/>
       <c r="C29" s="14"/>
@@ -2287,7 +2399,7 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A30" s="9"/>
       <c r="B30" s="8"/>
       <c r="C30" s="14"/>
@@ -2332,7 +2444,7 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A31" s="9"/>
       <c r="B31" s="8"/>
       <c r="C31" s="14"/>
@@ -2377,7 +2489,7 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A32" s="9"/>
       <c r="B32" s="8"/>
       <c r="C32" s="14"/>
@@ -2422,7 +2534,7 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A33" s="9"/>
       <c r="B33" s="8"/>
       <c r="C33" s="14"/>
@@ -2467,7 +2579,7 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="16"/>
@@ -2512,7 +2624,7 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="14.15">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -2557,52 +2669,52 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:43" customFormat="1"/>
+    <row r="37" spans="1:43" customFormat="1"/>
+    <row r="38" spans="1:43" customFormat="1"/>
+    <row r="39" spans="1:43" customFormat="1"/>
+    <row r="40" spans="1:43" customFormat="1"/>
+    <row r="41" spans="1:43" customFormat="1"/>
+    <row r="42" spans="1:43" customFormat="1"/>
+    <row r="43" spans="1:43" customFormat="1"/>
+    <row r="44" spans="1:43" customFormat="1"/>
+    <row r="45" spans="1:43" customFormat="1"/>
+    <row r="46" spans="1:43" customFormat="1"/>
+    <row r="47" spans="1:43" customFormat="1"/>
+    <row r="48" spans="1:43" customFormat="1"/>
+    <row r="49" customFormat="1"/>
+    <row r="50" customFormat="1"/>
+    <row r="51" customFormat="1"/>
+    <row r="52" customFormat="1"/>
+    <row r="53" customFormat="1"/>
+    <row r="54" customFormat="1"/>
+    <row r="55" customFormat="1"/>
+    <row r="56" customFormat="1"/>
+    <row r="57" customFormat="1"/>
+    <row r="58" customFormat="1"/>
+    <row r="59" customFormat="1"/>
+    <row r="60" customFormat="1"/>
+    <row r="61" customFormat="1"/>
+    <row r="62" customFormat="1"/>
+    <row r="63" customFormat="1"/>
+    <row r="64" customFormat="1"/>
+    <row r="65" customFormat="1"/>
+    <row r="66" customFormat="1"/>
+    <row r="67" customFormat="1"/>
+    <row r="68" customFormat="1"/>
+    <row r="69" customFormat="1"/>
+    <row r="70" customFormat="1"/>
+    <row r="71" customFormat="1"/>
+    <row r="72" customFormat="1"/>
+    <row r="73" customFormat="1"/>
+    <row r="74" customFormat="1"/>
+    <row r="75" customFormat="1"/>
+    <row r="76" customFormat="1"/>
+    <row r="77" customFormat="1"/>
+    <row r="78" customFormat="1"/>
+    <row r="79" customFormat="1"/>
+    <row r="80" customFormat="1"/>
+    <row r="81" customFormat="1"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="G1:H1"/>

</xml_diff>